<commit_message>
updated script and sample data
</commit_message>
<xml_diff>
--- a/sample data .xlsx
+++ b/sample data .xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\Python\excel-to-tally-automation-using-python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC2F2105-DD6E-4901-A0E6-FAF2CA8821C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C655074F-008E-49EF-8DA7-5E389F548E7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4944" yWindow="1200" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -180,10 +180,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -523,10 +527,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -558,7 +562,7 @@
       <c r="B2" t="s">
         <v>14</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="3">
         <v>15000</v>
       </c>
       <c r="D2" t="s">
@@ -572,7 +576,7 @@
       <c r="B3" t="s">
         <v>15</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="3">
         <v>25000</v>
       </c>
       <c r="D3" t="s">
@@ -586,7 +590,7 @@
       <c r="B4" t="s">
         <v>16</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="3">
         <v>18000</v>
       </c>
       <c r="D4" t="s">
@@ -600,7 +604,7 @@
       <c r="B5" t="s">
         <v>17</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="3">
         <v>22000</v>
       </c>
       <c r="D5" t="s">
@@ -614,7 +618,7 @@
       <c r="B6" t="s">
         <v>18</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="3">
         <v>32000</v>
       </c>
       <c r="D6" t="s">
@@ -628,7 +632,7 @@
       <c r="B7" t="s">
         <v>19</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="3">
         <v>29000</v>
       </c>
       <c r="D7" t="s">
@@ -642,7 +646,7 @@
       <c r="B8" t="s">
         <v>20</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="3">
         <v>14000</v>
       </c>
       <c r="D8" t="s">
@@ -656,7 +660,7 @@
       <c r="B9" t="s">
         <v>21</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="3">
         <v>41000</v>
       </c>
       <c r="D9" t="s">
@@ -670,7 +674,7 @@
       <c r="B10" t="s">
         <v>22</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="3">
         <v>50000</v>
       </c>
       <c r="D10" t="s">
@@ -684,12 +688,27 @@
       <c r="B11" t="s">
         <v>23</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="3">
         <v>12000</v>
       </c>
       <c r="D11" t="s">
         <v>33</v>
       </c>
+    </row>
+    <row r="20" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E20" s="2"/>
+    </row>
+    <row r="25" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E25" s="2"/>
+    </row>
+    <row r="30" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E30" s="2"/>
+    </row>
+    <row r="35" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E35" s="2"/>
+    </row>
+    <row r="44" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E44" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>